<commit_message>
Refactor and other implementation
</commit_message>
<xml_diff>
--- a/Example/Template.xlsx
+++ b/Example/Template.xlsx
@@ -80,7 +80,7 @@
     <t xml:space="preserve"> EFFETTUATO PRESSO IL VS CONDOMINIO </t>
   </si>
   <si>
-    <t>SERVIZIO DI TRASPORTO BIDONI  EFFETTUATO</t>
+    <t>SERVIZIO DI MANUTENZIONE E/O TRAPSORTO  EFFETTUATO</t>
   </si>
 </sst>
 </file>
@@ -1118,25 +1118,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -1149,239 +1130,40 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="22" fontId="8" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="22" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="22" fontId="8" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1417,26 +1199,244 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="22" fontId="8" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="22" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="22" fontId="8" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1811,7 +1811,7 @@
   <dimension ref="B1:N61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16:E16"/>
+      <selection activeCell="C17" sqref="C17:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1830,20 +1830,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" ht="121.5" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="F1" s="116"/>
-      <c r="G1" s="117"/>
-      <c r="H1" s="118"/>
+      <c r="F1" s="101"/>
+      <c r="G1" s="102"/>
+      <c r="H1" s="103"/>
       <c r="I1" s="45"/>
-      <c r="J1" s="115"/>
-      <c r="K1" s="115"/>
-      <c r="L1" s="115"/>
+      <c r="J1" s="100"/>
+      <c r="K1" s="100"/>
+      <c r="L1" s="100"/>
       <c r="M1" s="46"/>
       <c r="N1" s="42"/>
     </row>
     <row r="2" spans="2:14" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="F2" s="119"/>
-      <c r="G2" s="120"/>
-      <c r="H2" s="121"/>
+      <c r="F2" s="104"/>
+      <c r="G2" s="105"/>
+      <c r="H2" s="106"/>
       <c r="I2" s="13"/>
       <c r="J2" s="13"/>
       <c r="K2" s="14"/>
@@ -1903,11 +1903,11 @@
       <c r="C7" s="48"/>
       <c r="D7" s="12"/>
       <c r="E7" s="18"/>
-      <c r="F7" s="136"/>
-      <c r="G7" s="137"/>
-      <c r="H7" s="137"/>
-      <c r="I7" s="137"/>
-      <c r="J7" s="138"/>
+      <c r="F7" s="118"/>
+      <c r="G7" s="119"/>
+      <c r="H7" s="119"/>
+      <c r="I7" s="119"/>
+      <c r="J7" s="120"/>
       <c r="K7" s="42"/>
     </row>
     <row r="8" spans="2:14" ht="28.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.6">
@@ -1917,11 +1917,11 @@
       <c r="E8" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="133"/>
-      <c r="G8" s="134"/>
-      <c r="H8" s="134"/>
-      <c r="I8" s="134"/>
-      <c r="J8" s="135"/>
+      <c r="F8" s="115"/>
+      <c r="G8" s="116"/>
+      <c r="H8" s="116"/>
+      <c r="I8" s="116"/>
+      <c r="J8" s="117"/>
       <c r="K8" s="42"/>
     </row>
     <row r="9" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.6">
@@ -1930,53 +1930,53 @@
       </c>
       <c r="D9" s="75"/>
       <c r="E9" s="33"/>
-      <c r="F9" s="133"/>
-      <c r="G9" s="134"/>
-      <c r="H9" s="134"/>
-      <c r="I9" s="134"/>
-      <c r="J9" s="135"/>
+      <c r="F9" s="115"/>
+      <c r="G9" s="116"/>
+      <c r="H9" s="116"/>
+      <c r="I9" s="116"/>
+      <c r="J9" s="117"/>
       <c r="K9" s="42"/>
     </row>
     <row r="10" spans="2:14" ht="38.25" customHeight="1" x14ac:dyDescent="0.6">
       <c r="C10" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="146"/>
-      <c r="E10" s="146"/>
-      <c r="F10" s="133"/>
-      <c r="G10" s="134"/>
-      <c r="H10" s="134"/>
-      <c r="I10" s="134"/>
-      <c r="J10" s="135"/>
+      <c r="D10" s="127"/>
+      <c r="E10" s="127"/>
+      <c r="F10" s="115"/>
+      <c r="G10" s="116"/>
+      <c r="H10" s="116"/>
+      <c r="I10" s="116"/>
+      <c r="J10" s="117"/>
       <c r="K10" s="42"/>
     </row>
     <row r="11" spans="2:14" ht="33.6" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="C11" s="139"/>
-      <c r="D11" s="140"/>
-      <c r="E11" s="140"/>
-      <c r="F11" s="130"/>
-      <c r="G11" s="131"/>
-      <c r="H11" s="131"/>
-      <c r="I11" s="131"/>
-      <c r="J11" s="132"/>
+      <c r="C11" s="121"/>
+      <c r="D11" s="122"/>
+      <c r="E11" s="122"/>
+      <c r="F11" s="112"/>
+      <c r="G11" s="113"/>
+      <c r="H11" s="113"/>
+      <c r="I11" s="113"/>
+      <c r="J11" s="114"/>
       <c r="K11" s="66"/>
     </row>
     <row r="12" spans="2:14" ht="30.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C12" s="141"/>
-      <c r="D12" s="142"/>
-      <c r="E12" s="142"/>
+      <c r="C12" s="123"/>
+      <c r="D12" s="124"/>
+      <c r="E12" s="124"/>
       <c r="F12" s="73"/>
-      <c r="G12" s="150"/>
-      <c r="H12" s="150"/>
-      <c r="I12" s="150"/>
+      <c r="G12" s="92"/>
+      <c r="H12" s="92"/>
+      <c r="I12" s="92"/>
       <c r="J12" s="74"/>
     </row>
     <row r="13" spans="2:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="122" t="s">
+      <c r="C13" s="107" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="123"/>
-      <c r="E13" s="123"/>
+      <c r="D13" s="108"/>
+      <c r="E13" s="108"/>
       <c r="F13" s="70" t="s">
         <v>5</v>
       </c>
@@ -1991,9 +1991,9 @@
       <c r="K13" s="28"/>
     </row>
     <row r="14" spans="2:14" ht="27.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="147"/>
-      <c r="D14" s="148"/>
-      <c r="E14" s="149"/>
+      <c r="C14" s="89"/>
+      <c r="D14" s="90"/>
+      <c r="E14" s="91"/>
       <c r="F14" s="40"/>
       <c r="G14" s="35"/>
       <c r="H14" s="37"/>
@@ -2002,9 +2002,9 @@
       <c r="K14" s="29"/>
     </row>
     <row r="15" spans="2:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="127"/>
-      <c r="D15" s="128"/>
-      <c r="E15" s="129"/>
+      <c r="C15" s="109"/>
+      <c r="D15" s="110"/>
+      <c r="E15" s="111"/>
       <c r="F15" s="40"/>
       <c r="G15" s="35"/>
       <c r="H15" s="37"/>
@@ -2013,11 +2013,11 @@
       <c r="K15" s="29"/>
     </row>
     <row r="16" spans="2:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="143" t="s">
+      <c r="C16" s="125" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="144"/>
-      <c r="E16" s="145"/>
+      <c r="D16" s="82"/>
+      <c r="E16" s="126"/>
       <c r="F16" s="69" t="s">
         <v>11</v>
       </c>
@@ -2030,11 +2030,11 @@
       <c r="K16" s="29"/>
     </row>
     <row r="17" spans="3:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="124" t="s">
+      <c r="C17" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="144"/>
-      <c r="E17" s="158"/>
+      <c r="D17" s="82"/>
+      <c r="E17" s="83"/>
       <c r="F17" s="69"/>
       <c r="G17" s="25"/>
       <c r="H17" s="22"/>
@@ -2043,11 +2043,11 @@
       <c r="K17" s="29"/>
     </row>
     <row r="18" spans="3:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="124" t="s">
+      <c r="C18" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="125"/>
-      <c r="E18" s="126"/>
+      <c r="D18" s="80"/>
+      <c r="E18" s="81"/>
       <c r="F18" s="69"/>
       <c r="G18" s="25"/>
       <c r="H18" s="22"/>
@@ -2056,9 +2056,9 @@
       <c r="K18" s="29"/>
     </row>
     <row r="19" spans="3:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="124"/>
-      <c r="D19" s="125"/>
-      <c r="E19" s="126"/>
+      <c r="C19" s="79"/>
+      <c r="D19" s="80"/>
+      <c r="E19" s="81"/>
       <c r="F19" s="41"/>
       <c r="G19" s="25"/>
       <c r="H19" s="22"/>
@@ -2067,9 +2067,9 @@
       <c r="K19" s="29"/>
     </row>
     <row r="20" spans="3:11" ht="28.2" x14ac:dyDescent="0.25">
-      <c r="C20" s="161"/>
-      <c r="D20" s="144"/>
-      <c r="E20" s="158"/>
+      <c r="C20" s="86"/>
+      <c r="D20" s="82"/>
+      <c r="E20" s="83"/>
       <c r="F20" s="41"/>
       <c r="G20" s="25"/>
       <c r="H20" s="22"/>
@@ -2078,9 +2078,9 @@
       <c r="K20" s="29"/>
     </row>
     <row r="21" spans="3:11" ht="28.2" x14ac:dyDescent="0.25">
-      <c r="C21" s="161"/>
-      <c r="D21" s="162"/>
-      <c r="E21" s="158"/>
+      <c r="C21" s="86"/>
+      <c r="D21" s="87"/>
+      <c r="E21" s="83"/>
       <c r="F21" s="41"/>
       <c r="G21" s="25"/>
       <c r="H21" s="22"/>
@@ -2091,9 +2091,9 @@
       <c r="K21" s="29"/>
     </row>
     <row r="22" spans="3:11" ht="28.2" x14ac:dyDescent="0.25">
-      <c r="C22" s="82"/>
-      <c r="D22" s="83"/>
-      <c r="E22" s="84"/>
+      <c r="C22" s="76"/>
+      <c r="D22" s="77"/>
+      <c r="E22" s="78"/>
       <c r="F22" s="41"/>
       <c r="G22" s="25"/>
       <c r="H22" s="22"/>
@@ -2104,9 +2104,9 @@
       <c r="K22" s="29"/>
     </row>
     <row r="23" spans="3:11" ht="28.2" x14ac:dyDescent="0.25">
-      <c r="C23" s="82"/>
-      <c r="D23" s="83"/>
-      <c r="E23" s="84"/>
+      <c r="C23" s="76"/>
+      <c r="D23" s="77"/>
+      <c r="E23" s="78"/>
       <c r="F23" s="41"/>
       <c r="G23" s="25"/>
       <c r="H23" s="22"/>
@@ -2117,9 +2117,9 @@
       <c r="K23" s="29"/>
     </row>
     <row r="24" spans="3:11" ht="28.2" x14ac:dyDescent="0.25">
-      <c r="C24" s="82"/>
-      <c r="D24" s="83"/>
-      <c r="E24" s="84"/>
+      <c r="C24" s="76"/>
+      <c r="D24" s="77"/>
+      <c r="E24" s="78"/>
       <c r="F24" s="41"/>
       <c r="G24" s="25"/>
       <c r="H24" s="22"/>
@@ -2128,9 +2128,9 @@
       <c r="K24" s="29"/>
     </row>
     <row r="25" spans="3:11" ht="28.2" x14ac:dyDescent="0.25">
-      <c r="C25" s="82"/>
-      <c r="D25" s="83"/>
-      <c r="E25" s="84"/>
+      <c r="C25" s="76"/>
+      <c r="D25" s="77"/>
+      <c r="E25" s="78"/>
       <c r="F25" s="41"/>
       <c r="G25" s="25"/>
       <c r="H25" s="22"/>
@@ -2139,9 +2139,9 @@
       <c r="K25" s="29"/>
     </row>
     <row r="26" spans="3:11" ht="28.2" x14ac:dyDescent="0.25">
-      <c r="C26" s="82"/>
-      <c r="D26" s="83"/>
-      <c r="E26" s="84"/>
+      <c r="C26" s="76"/>
+      <c r="D26" s="77"/>
+      <c r="E26" s="78"/>
       <c r="F26" s="41"/>
       <c r="G26" s="25"/>
       <c r="H26" s="22"/>
@@ -2150,9 +2150,9 @@
       <c r="K26" s="29"/>
     </row>
     <row r="27" spans="3:11" ht="28.2" x14ac:dyDescent="0.25">
-      <c r="C27" s="82"/>
-      <c r="D27" s="83"/>
-      <c r="E27" s="84"/>
+      <c r="C27" s="76"/>
+      <c r="D27" s="77"/>
+      <c r="E27" s="78"/>
       <c r="F27" s="41"/>
       <c r="G27" s="25"/>
       <c r="H27" s="22"/>
@@ -2161,9 +2161,9 @@
       <c r="K27" s="29"/>
     </row>
     <row r="28" spans="3:11" ht="28.2" x14ac:dyDescent="0.25">
-      <c r="C28" s="82"/>
-      <c r="D28" s="83"/>
-      <c r="E28" s="84"/>
+      <c r="C28" s="76"/>
+      <c r="D28" s="77"/>
+      <c r="E28" s="78"/>
       <c r="F28" s="41"/>
       <c r="G28" s="25"/>
       <c r="H28" s="22"/>
@@ -2172,9 +2172,9 @@
       <c r="K28" s="29"/>
     </row>
     <row r="29" spans="3:11" ht="28.2" x14ac:dyDescent="0.25">
-      <c r="C29" s="82"/>
-      <c r="D29" s="83"/>
-      <c r="E29" s="84"/>
+      <c r="C29" s="76"/>
+      <c r="D29" s="77"/>
+      <c r="E29" s="78"/>
       <c r="F29" s="41"/>
       <c r="G29" s="25"/>
       <c r="H29" s="22"/>
@@ -2183,9 +2183,9 @@
       <c r="K29" s="29"/>
     </row>
     <row r="30" spans="3:11" ht="28.2" x14ac:dyDescent="0.25">
-      <c r="C30" s="82"/>
-      <c r="D30" s="83"/>
-      <c r="E30" s="84"/>
+      <c r="C30" s="76"/>
+      <c r="D30" s="77"/>
+      <c r="E30" s="78"/>
       <c r="F30" s="41"/>
       <c r="G30" s="25"/>
       <c r="H30" s="22"/>
@@ -2194,9 +2194,9 @@
       <c r="K30" s="29"/>
     </row>
     <row r="31" spans="3:11" ht="28.2" x14ac:dyDescent="0.25">
-      <c r="C31" s="82"/>
-      <c r="D31" s="83"/>
-      <c r="E31" s="84"/>
+      <c r="C31" s="76"/>
+      <c r="D31" s="77"/>
+      <c r="E31" s="78"/>
       <c r="F31" s="41"/>
       <c r="G31" s="25"/>
       <c r="H31" s="22"/>
@@ -2205,9 +2205,9 @@
       <c r="K31" s="29"/>
     </row>
     <row r="32" spans="3:11" ht="28.2" x14ac:dyDescent="0.25">
-      <c r="C32" s="82"/>
-      <c r="D32" s="83"/>
-      <c r="E32" s="84"/>
+      <c r="C32" s="76"/>
+      <c r="D32" s="77"/>
+      <c r="E32" s="78"/>
       <c r="F32" s="41"/>
       <c r="G32" s="25"/>
       <c r="H32" s="22"/>
@@ -2216,9 +2216,9 @@
       <c r="K32" s="29"/>
     </row>
     <row r="33" spans="3:11" ht="28.2" x14ac:dyDescent="0.25">
-      <c r="C33" s="82"/>
-      <c r="D33" s="83"/>
-      <c r="E33" s="84"/>
+      <c r="C33" s="76"/>
+      <c r="D33" s="77"/>
+      <c r="E33" s="78"/>
       <c r="F33" s="41"/>
       <c r="G33" s="25"/>
       <c r="H33" s="22"/>
@@ -2227,9 +2227,9 @@
       <c r="K33" s="29"/>
     </row>
     <row r="34" spans="3:11" ht="28.2" x14ac:dyDescent="0.25">
-      <c r="C34" s="82"/>
-      <c r="D34" s="83"/>
-      <c r="E34" s="84"/>
+      <c r="C34" s="76"/>
+      <c r="D34" s="77"/>
+      <c r="E34" s="78"/>
       <c r="F34" s="41"/>
       <c r="G34" s="25"/>
       <c r="H34" s="22"/>
@@ -2238,9 +2238,9 @@
       <c r="K34" s="29"/>
     </row>
     <row r="35" spans="3:11" ht="28.2" x14ac:dyDescent="0.25">
-      <c r="C35" s="82"/>
-      <c r="D35" s="83"/>
-      <c r="E35" s="84"/>
+      <c r="C35" s="76"/>
+      <c r="D35" s="77"/>
+      <c r="E35" s="78"/>
       <c r="F35" s="41"/>
       <c r="G35" s="25"/>
       <c r="H35" s="22"/>
@@ -2249,9 +2249,9 @@
       <c r="K35" s="29"/>
     </row>
     <row r="36" spans="3:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C36" s="82"/>
-      <c r="D36" s="83"/>
-      <c r="E36" s="84"/>
+      <c r="C36" s="76"/>
+      <c r="D36" s="77"/>
+      <c r="E36" s="78"/>
       <c r="F36" s="41"/>
       <c r="G36" s="25"/>
       <c r="H36" s="22"/>
@@ -2263,9 +2263,9 @@
       <c r="K36" s="29"/>
     </row>
     <row r="37" spans="3:11" ht="28.2" x14ac:dyDescent="0.35">
-      <c r="C37" s="155"/>
-      <c r="D37" s="156"/>
-      <c r="E37" s="157"/>
+      <c r="C37" s="97"/>
+      <c r="D37" s="98"/>
+      <c r="E37" s="99"/>
       <c r="F37" s="41"/>
       <c r="G37" s="25"/>
       <c r="H37" s="22"/>
@@ -2277,9 +2277,9 @@
       <c r="K37" s="29"/>
     </row>
     <row r="38" spans="3:11" ht="28.2" x14ac:dyDescent="0.25">
-      <c r="C38" s="82"/>
-      <c r="D38" s="83"/>
-      <c r="E38" s="84"/>
+      <c r="C38" s="76"/>
+      <c r="D38" s="77"/>
+      <c r="E38" s="78"/>
       <c r="F38" s="41"/>
       <c r="G38" s="25"/>
       <c r="H38" s="22"/>
@@ -2291,9 +2291,9 @@
       <c r="K38" s="29"/>
     </row>
     <row r="39" spans="3:11" ht="28.8" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C39" s="85"/>
-      <c r="D39" s="86"/>
-      <c r="E39" s="87"/>
+      <c r="C39" s="134"/>
+      <c r="D39" s="135"/>
+      <c r="E39" s="136"/>
       <c r="F39" s="41"/>
       <c r="G39" s="25"/>
       <c r="H39" s="22"/>
@@ -2305,9 +2305,9 @@
       <c r="K39" s="29"/>
     </row>
     <row r="40" spans="3:11" ht="28.8" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C40" s="88"/>
-      <c r="D40" s="89"/>
-      <c r="E40" s="90"/>
+      <c r="C40" s="137"/>
+      <c r="D40" s="138"/>
+      <c r="E40" s="139"/>
       <c r="F40" s="41"/>
       <c r="G40" s="25"/>
       <c r="H40" s="22"/>
@@ -2319,9 +2319,9 @@
       <c r="K40" s="29"/>
     </row>
     <row r="41" spans="3:11" ht="28.2" x14ac:dyDescent="0.25">
-      <c r="C41" s="82"/>
-      <c r="D41" s="83"/>
-      <c r="E41" s="84"/>
+      <c r="C41" s="76"/>
+      <c r="D41" s="77"/>
+      <c r="E41" s="78"/>
       <c r="F41" s="41"/>
       <c r="G41" s="25"/>
       <c r="H41" s="22"/>
@@ -2333,9 +2333,9 @@
       <c r="K41" s="29"/>
     </row>
     <row r="42" spans="3:11" ht="28.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C42" s="98"/>
-      <c r="D42" s="99"/>
-      <c r="E42" s="100"/>
+      <c r="C42" s="147"/>
+      <c r="D42" s="148"/>
+      <c r="E42" s="149"/>
       <c r="F42" s="41"/>
       <c r="G42" s="25"/>
       <c r="H42" s="22"/>
@@ -2347,9 +2347,9 @@
       <c r="K42" s="29"/>
     </row>
     <row r="43" spans="3:11" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C43" s="98"/>
-      <c r="D43" s="99"/>
-      <c r="E43" s="99"/>
+      <c r="C43" s="147"/>
+      <c r="D43" s="148"/>
+      <c r="E43" s="148"/>
       <c r="F43" s="21"/>
       <c r="G43" s="26"/>
       <c r="H43" s="24"/>
@@ -2361,9 +2361,9 @@
       <c r="K43" s="29"/>
     </row>
     <row r="44" spans="3:11" ht="24.6" x14ac:dyDescent="0.25">
-      <c r="C44" s="96"/>
-      <c r="D44" s="97"/>
-      <c r="E44" s="97"/>
+      <c r="C44" s="145"/>
+      <c r="D44" s="146"/>
+      <c r="E44" s="146"/>
       <c r="F44" s="9"/>
       <c r="G44" s="9"/>
       <c r="H44" s="10"/>
@@ -2379,9 +2379,9 @@
       <c r="D45" s="66"/>
       <c r="E45" s="32"/>
       <c r="F45" s="39"/>
-      <c r="G45" s="152"/>
-      <c r="H45" s="153"/>
-      <c r="I45" s="153"/>
+      <c r="G45" s="94"/>
+      <c r="H45" s="95"/>
+      <c r="I45" s="95"/>
       <c r="J45" s="51"/>
       <c r="K45" s="2"/>
     </row>
@@ -2390,15 +2390,15 @@
       <c r="D46" s="66"/>
       <c r="E46" s="32"/>
       <c r="F46" s="39"/>
-      <c r="G46" s="153"/>
-      <c r="H46" s="153"/>
-      <c r="I46" s="153"/>
+      <c r="G46" s="95"/>
+      <c r="H46" s="95"/>
+      <c r="I46" s="95"/>
       <c r="J46" s="51"/>
     </row>
     <row r="47" spans="3:11" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="C47" s="56"/>
-      <c r="D47" s="163"/>
-      <c r="E47" s="163"/>
+      <c r="D47" s="88"/>
+      <c r="E47" s="88"/>
       <c r="F47" s="39"/>
       <c r="G47" s="39"/>
       <c r="H47" s="32"/>
@@ -2407,43 +2407,43 @@
     </row>
     <row r="48" spans="3:11" ht="33" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="C48" s="57"/>
-      <c r="D48" s="101"/>
-      <c r="E48" s="102"/>
+      <c r="D48" s="150"/>
+      <c r="E48" s="151"/>
       <c r="F48" s="4"/>
       <c r="G48" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H48" s="80">
+      <c r="H48" s="132">
         <f>SUM(I14:I43)</f>
         <v>0</v>
       </c>
-      <c r="I48" s="81"/>
-      <c r="J48" s="81"/>
+      <c r="I48" s="133"/>
+      <c r="J48" s="133"/>
     </row>
     <row r="49" spans="3:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="C49" s="58"/>
-      <c r="D49" s="103"/>
-      <c r="E49" s="104"/>
+      <c r="D49" s="152"/>
+      <c r="E49" s="153"/>
       <c r="F49" s="5"/>
       <c r="G49" s="5"/>
-      <c r="H49" s="91"/>
-      <c r="I49" s="92"/>
-      <c r="J49" s="92"/>
+      <c r="H49" s="140"/>
+      <c r="I49" s="141"/>
+      <c r="J49" s="141"/>
     </row>
     <row r="50" spans="3:11" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
       <c r="C50" s="58"/>
-      <c r="D50" s="105"/>
-      <c r="E50" s="106"/>
+      <c r="D50" s="154"/>
+      <c r="E50" s="155"/>
       <c r="F50" s="5"/>
       <c r="G50" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="H50" s="159">
+      <c r="H50" s="84">
         <f>SUM(I14:I43)</f>
         <v>0</v>
       </c>
-      <c r="I50" s="160"/>
-      <c r="J50" s="160"/>
+      <c r="I50" s="85"/>
+      <c r="J50" s="85"/>
     </row>
     <row r="51" spans="3:11" ht="27.6" x14ac:dyDescent="0.45">
       <c r="C51" s="59"/>
@@ -2458,8 +2458,8 @@
     </row>
     <row r="52" spans="3:11" ht="22.8" x14ac:dyDescent="0.4">
       <c r="C52" s="59"/>
-      <c r="D52" s="107"/>
-      <c r="E52" s="108"/>
+      <c r="D52" s="156"/>
+      <c r="E52" s="157"/>
       <c r="F52" s="7"/>
       <c r="G52" s="7"/>
       <c r="H52" s="32"/>
@@ -2469,14 +2469,14 @@
     </row>
     <row r="53" spans="3:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="C53" s="61"/>
-      <c r="D53" s="151"/>
-      <c r="E53" s="151"/>
+      <c r="D53" s="93"/>
+      <c r="E53" s="93"/>
       <c r="F53" s="8"/>
       <c r="G53" s="8"/>
-      <c r="H53" s="154" t="s">
+      <c r="H53" s="96" t="s">
         <v>8</v>
       </c>
-      <c r="I53" s="154"/>
+      <c r="I53" s="96"/>
       <c r="J53" s="60"/>
     </row>
     <row r="54" spans="3:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2485,8 +2485,8 @@
       <c r="E54" s="27"/>
       <c r="F54" s="7"/>
       <c r="G54" s="7"/>
-      <c r="H54" s="76"/>
-      <c r="I54" s="76"/>
+      <c r="H54" s="128"/>
+      <c r="I54" s="128"/>
       <c r="J54" s="60"/>
     </row>
     <row r="55" spans="3:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2500,48 +2500,48 @@
       <c r="J55" s="60"/>
     </row>
     <row r="56" spans="3:11" ht="33" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C56" s="93"/>
-      <c r="D56" s="94"/>
-      <c r="E56" s="94"/>
-      <c r="F56" s="94"/>
-      <c r="G56" s="94"/>
-      <c r="H56" s="94"/>
-      <c r="I56" s="94"/>
-      <c r="J56" s="95"/>
+      <c r="C56" s="142"/>
+      <c r="D56" s="143"/>
+      <c r="E56" s="143"/>
+      <c r="F56" s="143"/>
+      <c r="G56" s="143"/>
+      <c r="H56" s="143"/>
+      <c r="I56" s="143"/>
+      <c r="J56" s="144"/>
       <c r="K56" s="1"/>
     </row>
     <row r="57" spans="3:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C57" s="109"/>
-      <c r="D57" s="110"/>
-      <c r="E57" s="110"/>
-      <c r="F57" s="110"/>
-      <c r="G57" s="110"/>
-      <c r="H57" s="110"/>
-      <c r="I57" s="110"/>
-      <c r="J57" s="111"/>
+      <c r="C57" s="158"/>
+      <c r="D57" s="159"/>
+      <c r="E57" s="159"/>
+      <c r="F57" s="159"/>
+      <c r="G57" s="159"/>
+      <c r="H57" s="159"/>
+      <c r="I57" s="159"/>
+      <c r="J57" s="160"/>
       <c r="K57" s="1"/>
     </row>
     <row r="58" spans="3:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C58" s="112"/>
-      <c r="D58" s="113"/>
-      <c r="E58" s="113"/>
-      <c r="F58" s="113"/>
-      <c r="G58" s="113"/>
-      <c r="H58" s="113"/>
-      <c r="I58" s="113"/>
-      <c r="J58" s="114"/>
+      <c r="C58" s="161"/>
+      <c r="D58" s="162"/>
+      <c r="E58" s="162"/>
+      <c r="F58" s="162"/>
+      <c r="G58" s="162"/>
+      <c r="H58" s="162"/>
+      <c r="I58" s="162"/>
+      <c r="J58" s="163"/>
     </row>
     <row r="59" spans="3:11" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C59" s="77" t="s">
+      <c r="C59" s="129" t="s">
         <v>4</v>
       </c>
-      <c r="D59" s="78"/>
-      <c r="E59" s="78"/>
-      <c r="F59" s="78"/>
-      <c r="G59" s="78"/>
-      <c r="H59" s="78"/>
-      <c r="I59" s="78"/>
-      <c r="J59" s="79"/>
+      <c r="D59" s="130"/>
+      <c r="E59" s="130"/>
+      <c r="F59" s="130"/>
+      <c r="G59" s="130"/>
+      <c r="H59" s="130"/>
+      <c r="I59" s="130"/>
+      <c r="J59" s="131"/>
     </row>
     <row r="60" spans="3:11" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C60" s="59"/>
@@ -2565,45 +2565,6 @@
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="H50:J50"/>
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="C33:E33"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="G45:I46"/>
-    <mergeCell ref="H53:I53"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="C34:E34"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="F1:H2"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="F11:J11"/>
-    <mergeCell ref="F10:J10"/>
-    <mergeCell ref="F7:J9"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="D10:E10"/>
     <mergeCell ref="H54:I54"/>
     <mergeCell ref="C59:J59"/>
     <mergeCell ref="H48:J48"/>
@@ -2620,6 +2581,45 @@
     <mergeCell ref="D52:E52"/>
     <mergeCell ref="C57:J57"/>
     <mergeCell ref="C58:J58"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="F1:H2"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="F11:J11"/>
+    <mergeCell ref="F10:J10"/>
+    <mergeCell ref="F7:J9"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="G45:I46"/>
+    <mergeCell ref="H53:I53"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="H50:J50"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="C31:E31"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>